<commit_message>
update: checking data and calculate linear exgression
</commit_message>
<xml_diff>
--- a/LAN_4.xlsx
+++ b/LAN_4.xlsx
@@ -1,26 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DO_AN_CDT\THUC_NGHIEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mechartrocnics - Project\Mechatronics-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{930A920D-C094-4551-AA0C-B21577C5CA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
   </bookViews>
   <sheets>
     <sheet name="Sensor_Input_Data_4" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>kl-vat ValueY</t>
   </si>
@@ -69,11 +68,77 @@
   <si>
     <t>B</t>
   </si>
+  <si>
+    <t xml:space="preserve">Hồi quy tuyến tính </t>
+  </si>
+  <si>
+    <t>x*y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Tb x</t>
+  </si>
+  <si>
+    <t>Tb y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">a </t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Do hs góc &gt; 0 ==&gt; tỉ lệ theo chiều thuận</t>
+  </si>
+  <si>
+    <t>Sx</t>
+  </si>
+  <si>
+    <t>Sy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r </t>
+  </si>
+  <si>
+    <t xml:space="preserve">t </t>
+  </si>
+  <si>
+    <t>t(Student)</t>
+  </si>
+  <si>
+    <t>1%==&gt; 3.4995 2% ==&gt; 2.9979 5%==&gt; 2.3646</t>
+  </si>
+  <si>
+    <t>Do trị đối của t &gt; t(Student) ==&gt; Có mối tương quan</t>
+  </si>
+  <si>
+    <t>Zr</t>
+  </si>
+  <si>
+    <t>Za/2</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p1 </t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -612,6 +677,1467 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Giá trị đo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="b"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$F$69:$F$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1036</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2770</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1290</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Giá trị thực tế</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$G$69:$G$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-731839440"/>
+        <c:axId val="-731832368"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-731839440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-731832368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-731832368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-731839440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4586287" y="14058900"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4586287" y="14058900"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>319087</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4586287" y="14058900"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="131831" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6615112" y="15049500"/>
+              <a:ext cx="131831" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>∑</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="7" name="TextBox 6"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6615112" y="15049500"/>
+              <a:ext cx="131831" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="334707" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6700837" y="17325975"/>
+              <a:ext cx="334707" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>∑</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> x^2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="8" name="TextBox 7"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6700837" y="17325975"/>
+              <a:ext cx="334707" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>∑</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t> x^2</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -909,13 +2435,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L927"/>
+  <dimension ref="A1:N927"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="L70" sqref="L70"/>
+    <sheetView tabSelected="1" topLeftCell="E97" workbookViewId="0">
+      <selection activeCell="N114" sqref="N114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="38" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -1618,7 +3149,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65">
         <v>854</v>
@@ -1629,7 +3160,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66">
         <v>920</v>
@@ -1640,7 +3171,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67">
         <v>1016</v>
@@ -1654,7 +3185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68">
         <v>940</v>
@@ -1678,7 +3209,7 @@
         <v>1.0227084688227608</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69">
         <v>932</v>
@@ -1706,7 +3237,7 @@
         <v>162.44018273256779</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70">
         <v>903</v>
@@ -1727,7 +3258,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71">
         <v>897</v>
@@ -1748,7 +3279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72">
         <v>1013</v>
@@ -1769,7 +3300,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73">
         <v>1036</v>
@@ -1790,7 +3321,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74">
         <v>1016</v>
@@ -1811,7 +3342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75">
         <v>955</v>
@@ -1832,7 +3363,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76">
         <v>1039</v>
@@ -1853,7 +3384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77">
         <v>1105</v>
@@ -1874,7 +3405,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78">
         <v>1073</v>
@@ -1885,7 +3416,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79">
         <v>0</v>
@@ -1895,8 +3426,11 @@
         <v>0</v>
       </c>
       <c r="E79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M79" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80">
         <v>0</v>
@@ -1906,8 +3440,19 @@
         <v>0</v>
       </c>
       <c r="E80" s="1"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L80" t="s">
+        <v>17</v>
+      </c>
+      <c r="M80">
+        <f>F69*G69</f>
+        <v>1089018</v>
+      </c>
+      <c r="N80">
+        <f>SUM(M80:M88)</f>
+        <v>22728289</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81">
         <v>0</v>
@@ -1917,8 +3462,12 @@
         <v>0</v>
       </c>
       <c r="E81" s="1"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <f t="shared" ref="M81:M88" si="0">F70*G70</f>
+        <v>953946</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82">
         <v>0</v>
@@ -1928,8 +3477,12 @@
         <v>0</v>
       </c>
       <c r="E82" s="1"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M82">
+        <f t="shared" si="0"/>
+        <v>1276352</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
       <c r="B83">
         <v>0</v>
@@ -1939,8 +3492,12 @@
         <v>0</v>
       </c>
       <c r="E83" s="1"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M83">
+        <f t="shared" si="0"/>
+        <v>2603172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1"/>
       <c r="B84">
         <v>0</v>
@@ -1950,8 +3507,12 @@
         <v>0</v>
       </c>
       <c r="E84" s="1"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M84">
+        <f t="shared" si="0"/>
+        <v>3696000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1"/>
       <c r="B85">
         <v>0</v>
@@ -1961,8 +3522,12 @@
         <v>0</v>
       </c>
       <c r="E85" s="1"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M85">
+        <f t="shared" si="0"/>
+        <v>8298920</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1"/>
       <c r="B86">
         <v>0</v>
@@ -1972,8 +3537,12 @@
         <v>0</v>
       </c>
       <c r="E86" s="1"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M86">
+        <f t="shared" si="0"/>
+        <v>852605</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1"/>
       <c r="B87">
         <v>0</v>
@@ -1983,8 +3552,12 @@
         <v>0</v>
       </c>
       <c r="E87" s="1"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M87">
+        <f t="shared" si="0"/>
+        <v>1980150</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1"/>
       <c r="B88">
         <v>0</v>
@@ -1994,8 +3567,12 @@
         <v>0</v>
       </c>
       <c r="E88" s="1"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M88">
+        <f t="shared" si="0"/>
+        <v>1978126</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1"/>
       <c r="B89">
         <v>0</v>
@@ -2005,8 +3582,15 @@
         <v>0</v>
       </c>
       <c r="E89" s="1"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L89" t="s">
+        <v>18</v>
+      </c>
+      <c r="M89">
+        <f>COUNT(M80:M88)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1"/>
       <c r="B90">
         <v>0</v>
@@ -2016,8 +3600,15 @@
         <v>0</v>
       </c>
       <c r="E90" s="1"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L90" t="s">
+        <v>19</v>
+      </c>
+      <c r="M90">
+        <f>AVERAGE(F69:F77)</f>
+        <v>1384.8888888888889</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1"/>
       <c r="B91">
         <v>0</v>
@@ -2027,8 +3618,15 @@
         <v>0</v>
       </c>
       <c r="E91" s="1"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L91" t="s">
+        <v>20</v>
+      </c>
+      <c r="M91">
+        <f>AVERAGE(G69:G77)</f>
+        <v>1578.7777777777778</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1"/>
       <c r="B92">
         <v>0</v>
@@ -2038,8 +3636,16 @@
         <v>0</v>
       </c>
       <c r="E92" s="1"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M92">
+        <f>POWER(F69,2)</f>
+        <v>879844</v>
+      </c>
+      <c r="N92">
+        <f>SUM(M92:M100)</f>
+        <v>20243926</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
       <c r="B93">
         <v>0</v>
@@ -2049,8 +3655,12 @@
         <v>0</v>
       </c>
       <c r="E93" s="1"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M93">
+        <f t="shared" ref="M93:M102" si="1">POWER(F70,2)</f>
+        <v>879844</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1"/>
       <c r="B94">
         <v>0</v>
@@ -2060,8 +3670,12 @@
         <v>0</v>
       </c>
       <c r="E94" s="1"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M94">
+        <f t="shared" si="1"/>
+        <v>1073296</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
       <c r="B95">
         <v>0</v>
@@ -2071,8 +3685,12 @@
         <v>0</v>
       </c>
       <c r="E95" s="1"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M95">
+        <f t="shared" si="1"/>
+        <v>2301289</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
       <c r="B96">
         <v>0</v>
@@ -2082,8 +3700,12 @@
         <v>0</v>
       </c>
       <c r="E96" s="1"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M96">
+        <f t="shared" si="1"/>
+        <v>3415104</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
       <c r="B97">
         <v>0</v>
@@ -2093,8 +3715,12 @@
         <v>0</v>
       </c>
       <c r="E97" s="1"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M97">
+        <f t="shared" si="1"/>
+        <v>7672900</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1"/>
       <c r="B98">
         <v>0</v>
@@ -2104,8 +3730,12 @@
         <v>0</v>
       </c>
       <c r="E98" s="1"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M98">
+        <f t="shared" si="1"/>
+        <v>714025</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1"/>
       <c r="B99">
         <v>0</v>
@@ -2115,8 +3745,12 @@
         <v>0</v>
       </c>
       <c r="E99" s="1"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M99">
+        <f t="shared" si="1"/>
+        <v>1664100</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="B100">
         <v>0</v>
@@ -2126,8 +3760,12 @@
         <v>0</v>
       </c>
       <c r="E100" s="1"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M100">
+        <f>POWER(F77,2)</f>
+        <v>1643524</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="B101">
         <v>0</v>
@@ -2137,8 +3775,18 @@
         <v>0</v>
       </c>
       <c r="E101" s="1"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L101" t="s">
+        <v>21</v>
+      </c>
+      <c r="M101">
+        <f>((N80-M89*M90*M91)/(N92-M89*POWER(M90,2)))</f>
+        <v>1.0227084688227603</v>
+      </c>
+      <c r="N101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1"/>
       <c r="B102">
         <v>0</v>
@@ -2148,8 +3796,15 @@
         <v>0</v>
       </c>
       <c r="E102" s="1"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L102" t="s">
+        <v>22</v>
+      </c>
+      <c r="M102">
+        <f>M91-M101*M90</f>
+        <v>162.44018273256847</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
       <c r="B103">
         <v>0</v>
@@ -2159,8 +3814,15 @@
         <v>0</v>
       </c>
       <c r="E103" s="1"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L103" t="s">
+        <v>23</v>
+      </c>
+      <c r="M103">
+        <f>M101*1036+M102</f>
+        <v>1221.9661564329481</v>
+      </c>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="1"/>
       <c r="B104">
         <v>0</v>
@@ -2170,8 +3832,14 @@
         <v>0</v>
       </c>
       <c r="E104" s="1"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L104" t="s">
+        <v>25</v>
+      </c>
+      <c r="M104">
+        <v>610.60122920000003</v>
+      </c>
+    </row>
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="1"/>
       <c r="B105">
         <v>0</v>
@@ -2181,8 +3849,14 @@
         <v>0</v>
       </c>
       <c r="E105" s="1"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L105" t="s">
+        <v>26</v>
+      </c>
+      <c r="M105">
+        <v>626.79816879999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="1"/>
       <c r="B106">
         <v>0</v>
@@ -2192,8 +3866,14 @@
         <v>0</v>
       </c>
       <c r="E106" s="1"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L106" t="s">
+        <v>27</v>
+      </c>
+      <c r="M106">
+        <v>0.99628090709999995</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="1"/>
       <c r="B107">
         <v>0</v>
@@ -2203,8 +3883,14 @@
         <v>0</v>
       </c>
       <c r="E107" s="1"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L107" t="s">
+        <v>28</v>
+      </c>
+      <c r="M107">
+        <v>30.591549959999998</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108">
         <v>0</v>
@@ -2214,8 +3900,17 @@
         <v>0</v>
       </c>
       <c r="E108" s="1"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L108" t="s">
+        <v>29</v>
+      </c>
+      <c r="M108" t="s">
+        <v>30</v>
+      </c>
+      <c r="N108" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109">
         <v>0</v>
@@ -2225,8 +3920,14 @@
         <v>0</v>
       </c>
       <c r="E109" s="1"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L109" t="s">
+        <v>32</v>
+      </c>
+      <c r="M109">
+        <v>3.14278068</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110">
         <v>0</v>
@@ -2236,8 +3937,14 @@
         <v>0</v>
       </c>
       <c r="E110" s="1"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L110" t="s">
+        <v>33</v>
+      </c>
+      <c r="M110">
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111">
         <v>0</v>
@@ -2247,8 +3954,14 @@
         <v>0</v>
       </c>
       <c r="E111" s="1"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L111" t="s">
+        <v>34</v>
+      </c>
+      <c r="M111">
+        <v>2.3426140310000001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112">
         <v>0</v>
@@ -2258,8 +3971,14 @@
         <v>0</v>
       </c>
       <c r="E112" s="1"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L112" t="s">
+        <v>35</v>
+      </c>
+      <c r="M112">
+        <v>3.9429473289999999</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" s="1"/>
       <c r="B113">
         <v>0</v>
@@ -2269,8 +3988,14 @@
         <v>0</v>
       </c>
       <c r="E113" s="1"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L113" t="s">
+        <v>36</v>
+      </c>
+      <c r="M113">
+        <v>0.98170759200000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" s="1"/>
       <c r="B114">
         <v>0</v>
@@ -2280,8 +4005,14 @@
         <v>0</v>
       </c>
       <c r="E114" s="1"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="L114" t="s">
+        <v>37</v>
+      </c>
+      <c r="M114">
+        <v>0.99924826249999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" s="1"/>
       <c r="B115">
         <v>0</v>
@@ -2292,7 +4023,7 @@
       </c>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" s="1"/>
       <c r="B116">
         <v>0</v>
@@ -2303,7 +4034,7 @@
       </c>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
       <c r="B117">
         <v>0</v>
@@ -2314,7 +4045,7 @@
       </c>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
       <c r="B118">
         <v>0</v>
@@ -2325,7 +4056,7 @@
       </c>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" s="1"/>
       <c r="B119">
         <v>0</v>
@@ -2336,7 +4067,7 @@
       </c>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" s="1"/>
       <c r="B120">
         <v>0</v>
@@ -2347,7 +4078,7 @@
       </c>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" s="1"/>
       <c r="B121">
         <v>0</v>
@@ -2358,7 +4089,7 @@
       </c>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" s="1"/>
       <c r="B122">
         <v>0</v>
@@ -2369,7 +4100,7 @@
       </c>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
       <c r="B123">
         <v>0</v>
@@ -2380,7 +4111,7 @@
       </c>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" s="1"/>
       <c r="B124">
         <v>0</v>
@@ -2391,7 +4122,7 @@
       </c>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" s="1"/>
       <c r="B125">
         <v>0</v>
@@ -2402,7 +4133,7 @@
       </c>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" s="1"/>
       <c r="B126">
         <v>0</v>
@@ -2413,7 +4144,7 @@
       </c>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127">
         <v>0</v>
@@ -2424,7 +4155,7 @@
       </c>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128">
         <v>0</v>
@@ -11222,5 +12953,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update: update excel file
</commit_message>
<xml_diff>
--- a/LAN_4.xlsx
+++ b/LAN_4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>kl-vat ValueY</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>p2</t>
+  </si>
+  <si>
+    <t>Sau khi áp hàm bậc nhất</t>
   </si>
 </sst>
 </file>
@@ -992,11 +995,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-731839440"/>
-        <c:axId val="-731832368"/>
+        <c:axId val="1868864096"/>
+        <c:axId val="1868859744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-731839440"/>
+        <c:axId val="1868864096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1038,7 +1041,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-731832368"/>
+        <c:crossAx val="1868859744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1046,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-731832368"/>
+        <c:axId val="1868859744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1097,7 +1100,448 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-731839440"/>
+        <c:crossAx val="1868864096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Giá trị thực tế </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$M$68:$M$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1121.7407256839999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1121.7407256839999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1221.966155548</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1713.888928656</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2052.4054315640001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2995.3426390600002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1026.62883816</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1481.73410642</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1473.5524386760001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Giá trị cân sau áp hàm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$G$69:$G$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1929003856"/>
+        <c:axId val="1928972848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1929003856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1928972848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1928972848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1929003856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1218,7 +1662,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1908,8 +2895,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="131831" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -1945,6 +2932,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1966,7 +2954,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6"/>
@@ -2025,8 +3013,8 @@
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="334707" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -2081,7 +3069,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="TextBox 7"/>
@@ -2135,6 +3123,36 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2437,8 +3455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N927"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E97" workbookViewId="0">
-      <selection activeCell="N114" sqref="N114"/>
+    <sheetView tabSelected="1" topLeftCell="C102" workbookViewId="0">
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3184,6 +4202,9 @@
       <c r="K67" t="s">
         <v>13</v>
       </c>
+      <c r="M67" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
@@ -3208,6 +4229,10 @@
         <f>SLOPE(G69:G77,F69:F77)</f>
         <v>1.0227084688227608</v>
       </c>
+      <c r="M68">
+        <f>1.022708468*F69+162.4401827</f>
+        <v>1121.7407256839999</v>
+      </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
@@ -3236,6 +4261,10 @@
         <f>INTERCEPT(G69:G77,F69:F77)</f>
         <v>162.44018273256779</v>
       </c>
+      <c r="M69">
+        <f t="shared" ref="M69:M76" si="0">1.022708468*F70+162.4401827</f>
+        <v>1121.7407256839999</v>
+      </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
@@ -3257,6 +4286,10 @@
       <c r="H70" t="s">
         <v>3</v>
       </c>
+      <c r="M70">
+        <f t="shared" si="0"/>
+        <v>1221.966155548</v>
+      </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
@@ -3278,6 +4311,10 @@
       <c r="H71" t="s">
         <v>4</v>
       </c>
+      <c r="M71">
+        <f t="shared" si="0"/>
+        <v>1713.888928656</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
@@ -3299,6 +4336,10 @@
       <c r="H72" t="s">
         <v>5</v>
       </c>
+      <c r="M72">
+        <f t="shared" si="0"/>
+        <v>2052.4054315640001</v>
+      </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
@@ -3320,6 +4361,10 @@
       <c r="H73" t="s">
         <v>6</v>
       </c>
+      <c r="M73">
+        <f t="shared" si="0"/>
+        <v>2995.3426390600002</v>
+      </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
@@ -3341,6 +4386,10 @@
       <c r="H74" t="s">
         <v>7</v>
       </c>
+      <c r="M74">
+        <f t="shared" si="0"/>
+        <v>1026.62883816</v>
+      </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
@@ -3362,6 +4411,10 @@
       <c r="H75" t="s">
         <v>8</v>
       </c>
+      <c r="M75">
+        <f t="shared" si="0"/>
+        <v>1481.73410642</v>
+      </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
@@ -3383,6 +4436,10 @@
       <c r="H76" t="s">
         <v>9</v>
       </c>
+      <c r="M76">
+        <f t="shared" si="0"/>
+        <v>1473.5524386760001</v>
+      </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
@@ -3463,7 +4520,7 @@
       </c>
       <c r="E81" s="1"/>
       <c r="M81">
-        <f t="shared" ref="M81:M88" si="0">F70*G70</f>
+        <f t="shared" ref="M81:M88" si="1">F70*G70</f>
         <v>953946</v>
       </c>
     </row>
@@ -3478,7 +4535,7 @@
       </c>
       <c r="E82" s="1"/>
       <c r="M82">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1276352</v>
       </c>
     </row>
@@ -3493,7 +4550,7 @@
       </c>
       <c r="E83" s="1"/>
       <c r="M83">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2603172</v>
       </c>
     </row>
@@ -3508,7 +4565,7 @@
       </c>
       <c r="E84" s="1"/>
       <c r="M84">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3696000</v>
       </c>
     </row>
@@ -3523,7 +4580,7 @@
       </c>
       <c r="E85" s="1"/>
       <c r="M85">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8298920</v>
       </c>
     </row>
@@ -3538,7 +4595,7 @@
       </c>
       <c r="E86" s="1"/>
       <c r="M86">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>852605</v>
       </c>
     </row>
@@ -3553,7 +4610,7 @@
       </c>
       <c r="E87" s="1"/>
       <c r="M87">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1980150</v>
       </c>
     </row>
@@ -3568,7 +4625,7 @@
       </c>
       <c r="E88" s="1"/>
       <c r="M88">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1978126</v>
       </c>
     </row>
@@ -3656,7 +4713,7 @@
       </c>
       <c r="E93" s="1"/>
       <c r="M93">
-        <f t="shared" ref="M93:M102" si="1">POWER(F70,2)</f>
+        <f t="shared" ref="M93:M99" si="2">POWER(F70,2)</f>
         <v>879844</v>
       </c>
     </row>
@@ -3671,7 +4728,7 @@
       </c>
       <c r="E94" s="1"/>
       <c r="M94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1073296</v>
       </c>
     </row>
@@ -3686,7 +4743,7 @@
       </c>
       <c r="E95" s="1"/>
       <c r="M95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2301289</v>
       </c>
     </row>
@@ -3701,7 +4758,7 @@
       </c>
       <c r="E96" s="1"/>
       <c r="M96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3415104</v>
       </c>
     </row>
@@ -3716,7 +4773,7 @@
       </c>
       <c r="E97" s="1"/>
       <c r="M97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7672900</v>
       </c>
     </row>
@@ -3731,7 +4788,7 @@
       </c>
       <c r="E98" s="1"/>
       <c r="M98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>714025</v>
       </c>
     </row>
@@ -3746,7 +4803,7 @@
       </c>
       <c r="E99" s="1"/>
       <c r="M99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1664100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update: update some report
</commit_message>
<xml_diff>
--- a/LAN_4.xlsx
+++ b/LAN_4.xlsx
@@ -695,6 +695,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Giá</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> trị cân khi chưa qua xử lý</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -735,7 +765,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Giá trị đo</c:v>
+            <c:v>Giá trị cân trên băng tải</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -995,11 +1025,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1868864096"/>
-        <c:axId val="1868859744"/>
+        <c:axId val="-236302496"/>
+        <c:axId val="-234123744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1868864096"/>
+        <c:axId val="-236302496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1071,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868859744"/>
+        <c:crossAx val="-234123744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1079,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1868859744"/>
+        <c:axId val="-234123744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1100,7 +1130,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1868864096"/>
+        <c:crossAx val="-236302496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1196,6 +1226,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Giá trị cân sau khi áp dụng hàm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1436,11 +1496,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1929003856"/>
-        <c:axId val="1928972848"/>
+        <c:axId val="-234116128"/>
+        <c:axId val="-234123200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1929003856"/>
+        <c:axId val="-234116128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,7 +1542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1928972848"/>
+        <c:crossAx val="-234123200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1490,7 +1550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1928972848"/>
+        <c:axId val="-234123200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1929003856"/>
+        <c:crossAx val="-234116128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,6 +1682,366 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Scatter</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Diagram</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$F$69:$F$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>938</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1036</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1517</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1848</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2770</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1290</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1282</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sensor_Input_Data_4!$G$69:$G$77</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1716</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1535</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1543</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-120532640"/>
+        <c:axId val="-120537536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-120532640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-120537536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-120537536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-120532640"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1663,6 +2083,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2708,20 +3168,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>480128</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>144384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:colOff>176794</xdr:colOff>
       <xdr:row>93</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>30084</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3153,6 +4129,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3922</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>38002</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>272911</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>114202</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3455,8 +4461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N927"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C102" workbookViewId="0">
-      <selection activeCell="M111" sqref="M111"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>